<commit_message>
Updated Mar 25 2022
</commit_message>
<xml_diff>
--- a/table/Table_2.xlsx
+++ b/table/Table_2.xlsx
@@ -15,28 +15,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
-    <t>Panel A: Total Visits/Admissions</t>
-  </si>
-  <si>
-    <t>covid19</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Panel B: Infectious Diseases</t>
-  </si>
-  <si>
-    <t>covid19</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Panel C: Non-infectious diseases</t>
-  </si>
-  <si>
-    <t>covid19</t>
+    <t>\multicolumn{9}{@{}l@{}}{\textbf{Panel A:} All diseases}</t>
+  </si>
+  <si>
+    <t>$Y_{2020} \times Post$</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>\multicolumn{9}{@{}l@{}}{\textbf{Panel B:} ILI diseases}</t>
+  </si>
+  <si>
+    <t>$Y_{2020} \times Post$</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>\multicolumn{9}{@{}l@{}}{\textbf{Panel C:} Non-ILI diseases}</t>
+  </si>
+  <si>
+    <t>$Y_{2020} \times Post$</t>
   </si>
   <si>
     <t/>
@@ -48,40 +54,196 @@
     <t>Observations</t>
   </si>
   <si>
-    <t>Robust standard errors in parentheses</t>
-  </si>
-  <si>
-    <t>*** p&lt;0.01, ** p&lt;0.05, * p&lt;0.1</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.14***</t>
+    <t/>
+  </si>
+  <si>
+    <t>0.87***</t>
   </si>
   <si>
     <t>(0.01)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.44***</t>
+    <t>[0.86,0.89]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.63***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.59,0.68]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.90***</t>
+  </si>
+  <si>
+    <t>(0.00)</t>
+  </si>
+  <si>
+    <t>[0.89,0.91]</t>
+  </si>
+  <si>
+    <t>8,008</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.88***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.84,0.92]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.63***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.58,0.68]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.91***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.87,0.94]</t>
+  </si>
+  <si>
+    <t>8,008</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.87***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.84,0.90]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.62***</t>
   </si>
   <si>
     <t>(0.03)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.10***</t>
+    <t>[0.58,0.67]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.90***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.87,0.93]</t>
+  </si>
+  <si>
+    <t>8,008</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.87***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.84,0.90]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.62***</t>
+  </si>
+  <si>
+    <t>(0.03)</t>
+  </si>
+  <si>
+    <t>[0.57,0.67]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.90***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.87,0.93]</t>
+  </si>
+  <si>
+    <t>8,008</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.95***</t>
+  </si>
+  <si>
+    <t>(0.00)</t>
+  </si>
+  <si>
+    <t>[0.94,0.96]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.60***</t>
   </si>
   <si>
     <t>(0.01)</t>
   </si>
   <si>
-    <t/>
+    <t>[0.57,0.63]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.98***</t>
+  </si>
+  <si>
+    <t>(0.00)</t>
+  </si>
+  <si>
+    <t>[0.97,0.98]</t>
   </si>
   <si>
     <t>8,008</t>
@@ -90,37 +252,37 @@
     <t/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.14***</t>
+    <t>0.96**</t>
   </si>
   <si>
     <t>(0.01)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.45***</t>
+    <t>[0.94,0.99]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.60***</t>
   </si>
   <si>
     <t>(0.03)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.09***</t>
-  </si>
-  <si>
-    <t>(0.01)</t>
-  </si>
-  <si>
-    <t/>
+    <t>[0.54,0.65]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>[0.96,1.02]</t>
   </si>
   <si>
     <t>8,008</t>
@@ -129,37 +291,37 @@
     <t/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.14***</t>
-  </si>
-  <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.45***</t>
+    <t>0.95</t>
   </si>
   <si>
     <t>(0.03)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.10***</t>
-  </si>
-  <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t/>
+    <t>[0.90,1.01]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.60***</t>
+  </si>
+  <si>
+    <t>(0.04)</t>
+  </si>
+  <si>
+    <t>[0.53,0.68]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>(0.03)</t>
+  </si>
+  <si>
+    <t>[0.92,1.04]</t>
   </si>
   <si>
     <t>8,008</t>
@@ -168,202 +330,40 @@
     <t/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.14***</t>
-  </si>
-  <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.45***</t>
+    <t>0.96</t>
   </si>
   <si>
     <t>(0.03)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.10***</t>
-  </si>
-  <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t/>
+    <t>[0.90,1.01]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.60***</t>
+  </si>
+  <si>
+    <t>(0.04)</t>
+  </si>
+  <si>
+    <t>[0.54,0.68]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>(0.03)</t>
+  </si>
+  <si>
+    <t>[0.92,1.05]</t>
   </si>
   <si>
     <t>8,008</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.05***</t>
-  </si>
-  <si>
-    <t>(0.01)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.43***</t>
-  </si>
-  <si>
-    <t>(0.01)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.02***</t>
-  </si>
-  <si>
-    <t>(0.00)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>8,008</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.05***</t>
-  </si>
-  <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.47***</t>
-  </si>
-  <si>
-    <t>(0.04)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.02</t>
-  </si>
-  <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>8,008</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.05</t>
-  </si>
-  <si>
-    <t>(0.03)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.42***</t>
-  </si>
-  <si>
-    <t>(0.05)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.02</t>
-  </si>
-  <si>
-    <t>(0.03)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>8,008</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.04</t>
-  </si>
-  <si>
-    <t>(0.03)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.42***</t>
-  </si>
-  <si>
-    <t>(0.05)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-0.01</t>
-  </si>
-  <si>
-    <t>(0.04)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>8,008</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>

</xml_diff>